<commit_message>
Updated app.py with histogram and new Excel data
</commit_message>
<xml_diff>
--- a/test_report.xlsx
+++ b/test_report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cryan\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cryan\Documents\test_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95044F64-3950-4065-AC55-07D851D00517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39952218-A121-43EF-BF8E-A453ECDA2274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{B7D3E997-444B-4A00-AA7D-8D60383921B1}"/>
+    <workbookView xWindow="-6780" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{B7D3E997-444B-4A00-AA7D-8D60383921B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,31 +36,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Exposure</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Counterparty</t>
   </si>
   <si>
-    <t>BP</t>
-  </si>
-  <si>
-    <t>CNCRD</t>
-  </si>
-  <si>
-    <t>CIMA</t>
+    <t>CP_1</t>
+  </si>
+  <si>
+    <t>CP_2</t>
+  </si>
+  <si>
+    <t>CP_3</t>
+  </si>
+  <si>
+    <t>CP_4</t>
+  </si>
+  <si>
+    <t>CP_5</t>
+  </si>
+  <si>
+    <t>CP_6</t>
+  </si>
+  <si>
+    <t>CP_7</t>
+  </si>
+  <si>
+    <t>Available Credit</t>
+  </si>
+  <si>
+    <t>Utilization Rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +90,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,10 +125,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -105,12 +138,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -442,62 +482,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD0B79F-2DCD-4698-8796-E154CC70B8E7}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>12000</v>
       </c>
-      <c r="C2" s="3">
-        <v>45748</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C2" s="4">
+        <v>15000</v>
+      </c>
+      <c r="D2" s="6">
+        <f>B2/C2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>9500</v>
       </c>
-      <c r="C3" s="3">
-        <v>45749</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3" s="4">
+        <v>10000</v>
+      </c>
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:D8" si="0">B3/C3</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>15000</v>
       </c>
-      <c r="C4" s="3">
-        <v>45755</v>
+      <c r="C4" s="4">
+        <v>20000</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5000</v>
+      </c>
+      <c r="C5" s="5">
+        <v>10000</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C6" s="5">
+        <v>15000</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>10000</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3500</v>
+      </c>
+      <c r="C8" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>